<commit_message>
updated profiles.xlsx to reflect spend by day for picnic
</commit_message>
<xml_diff>
--- a/out/profiles.xlsx
+++ b/out/profiles.xlsx
@@ -8,16 +8,16 @@
     <sheet name="README" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="pop" sheetId="4" state="visible" r:id="rId2"/>
     <sheet name="cpi" sheetId="5" state="visible" r:id="rId3"/>
-    <sheet name="avgSpendPicnic" sheetId="18" state="visible" r:id="rId4"/>
-    <sheet name="spend" sheetId="19" state="visible" r:id="rId5"/>
-    <sheet name="spendAll" sheetId="20" state="visible" r:id="rId6"/>
+    <sheet name="avgSpendPicnic" sheetId="21" state="visible" r:id="rId4"/>
+    <sheet name="spend" sheetId="22" state="visible" r:id="rId5"/>
+    <sheet name="spendAll" sheetId="23" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="241">
   <si>
     <t>Picnic Average Spending: AZ 2018 survey</t>
   </si>
@@ -55,9 +55,6 @@
     <t>spend*</t>
   </si>
   <si>
-    <t>2018 Average annual spending (per participant) by item for picnicking</t>
-  </si>
-  <si>
     <t>spendAll*</t>
   </si>
   <si>
@@ -73,6 +70,27 @@
     <t>act</t>
   </si>
   <si>
+    <t>US Census &amp; BLS: Population and CPI used for adjusting to 2019</t>
+  </si>
+  <si>
+    <t>* Multiplying non-dimensional variables yields CO statewide spending along the water in 2019</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>act-type-item</t>
+  </si>
+  <si>
+    <t>act</t>
+  </si>
+  <si>
     <t>type</t>
   </si>
   <si>
@@ -394,22 +412,7 @@
     <t>othequip</t>
   </si>
   <si>
-    <t>US Census &amp; BLS: Population and CPI used for adjusting to 2019</t>
-  </si>
-  <si>
-    <t>* Multiplying non-dimensional variables yields CO statewide spending along the water in 2019</t>
-  </si>
-  <si>
-    <t>Tab</t>
-  </si>
-  <si>
-    <t>Dimensions</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>act-type-item</t>
+    <t>2018 Average annual spending (per day) by item for picnicking</t>
   </si>
   <si>
     <t xml:space="preserve">act</t>
@@ -434,6 +437,9 @@
   </si>
   <si>
     <t xml:space="preserve">waterRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avgDays</t>
   </si>
   <si>
     <t xml:space="preserve">waterShare</t>
@@ -1098,7 +1104,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
@@ -1128,25 +1134,25 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>125</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>127</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>128</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>129</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
@@ -1176,21 +1182,21 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
@@ -1198,15 +1204,15 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>126</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3"/>
     </row>
@@ -1386,45 +1392,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J1" t="s">
-        <v>140</v>
+        <v>141</v>
+      </c>
+      <c r="K1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D2" t="n">
         <v>22.1876386790728</v>
@@ -1442,21 +1451,24 @@
         <v>0.744512242290976</v>
       </c>
       <c r="I2" t="n">
+        <v>13.5999789482675</v>
+      </c>
+      <c r="J2" t="n">
         <v>0.539061763837546</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>1.01831939466348</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D3" t="n">
         <v>9.56018824107881</v>
@@ -1474,21 +1486,24 @@
         <v>0.744512242290976</v>
       </c>
       <c r="I3" t="n">
+        <v>13.5999789482675</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.539061763837546</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>1.01831939466348</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D4" t="n">
         <v>2.96856506157932</v>
@@ -1506,21 +1521,24 @@
         <v>0.744512242290976</v>
       </c>
       <c r="I4" t="n">
+        <v>13.5999789482675</v>
+      </c>
+      <c r="J4" t="n">
         <v>0.539061763837546</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>1.01831939466348</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D5" t="n">
         <v>19.6567297571605</v>
@@ -1538,9 +1556,12 @@
         <v>0.744512242290976</v>
       </c>
       <c r="I5" t="n">
+        <v>13.5999789482675</v>
+      </c>
+      <c r="J5" t="n">
         <v>0.539061763837546</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>1.01831939466348</v>
       </c>
     </row>
@@ -1560,39 +1581,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D2" t="n">
         <v>43346083.9822968</v>
@@ -1612,13 +1633,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D3" t="n">
         <v>660425578.686793</v>
@@ -1638,13 +1659,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D4" t="n">
         <v>193165839.744295</v>
@@ -1664,13 +1685,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D5" t="n">
         <v>222739390.824956</v>
@@ -1690,13 +1711,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D6" t="n">
         <v>140737931.350099</v>
@@ -1716,13 +1737,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D7" t="n">
         <v>445522386.948079</v>
@@ -1742,13 +1763,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" t="s">
         <v>152</v>
-      </c>
-      <c r="B8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" t="s">
-        <v>150</v>
       </c>
       <c r="D8" t="n">
         <v>37834500.7200707</v>
@@ -1768,13 +1789,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D9" t="n">
         <v>1215131403.20535</v>
@@ -1794,13 +1815,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D10" t="n">
         <v>629080357.561793</v>
@@ -1820,13 +1841,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D11" t="n">
         <v>29049513.6816096</v>
@@ -1846,13 +1867,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D12" t="n">
         <v>474629382.399854</v>
@@ -1872,13 +1893,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D13" t="n">
         <v>260000715.789691</v>
@@ -1898,13 +1919,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D14" t="n">
         <v>921301144.974733</v>
@@ -1924,13 +1945,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C15" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D15" t="n">
         <v>59031618.3724717</v>
@@ -1950,13 +1971,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D16" t="n">
         <v>1677509710.64684</v>
@@ -1976,13 +1997,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C17" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D17" t="n">
         <v>1761252210.34094</v>
@@ -2002,13 +2023,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C18" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D18" t="n">
         <v>1692462078.89392</v>
@@ -2028,13 +2049,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D19" t="n">
         <v>322257226.86143</v>
@@ -2054,13 +2075,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B20" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C20" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D20" t="n">
         <v>1450813926.22736</v>
@@ -2080,13 +2101,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B21" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C21" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D21" t="n">
         <v>139384576.520521</v>
@@ -2106,13 +2127,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B22" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C22" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D22" t="n">
         <v>1975681602.08825</v>
@@ -2132,13 +2153,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C23" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D23" t="n">
         <v>1150694572.86489</v>
@@ -2158,13 +2179,13 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B24" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C24" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D24" t="n">
         <v>937443008.033508</v>
@@ -2184,13 +2205,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B25" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C25" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D25" t="n">
         <v>518864193.263192</v>
@@ -2210,13 +2231,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B26" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C26" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D26" t="n">
         <v>1769063999.29467</v>
@@ -2236,13 +2257,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B27" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C27" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D27" t="n">
         <v>36746784.3351276</v>
@@ -2262,13 +2283,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B28" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C28" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D28" t="n">
         <v>514314437.647142</v>
@@ -2288,13 +2309,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B29" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C29" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D29" t="n">
         <v>315627121.013466</v>
@@ -2314,13 +2335,13 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C30" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D30" t="n">
         <v>16197565.7054073</v>
@@ -2340,13 +2361,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C31" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D31" t="n">
         <v>300634539.975694</v>
@@ -2366,13 +2387,13 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B32" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C32" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D32" t="n">
         <v>102068772.545705</v>
@@ -2392,13 +2413,13 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C33" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D33" t="n">
         <v>410864297.754511</v>
@@ -2418,13 +2439,13 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B34" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C34" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D34" t="n">
         <v>30500851.3832994</v>
@@ -2444,13 +2465,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B35" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C35" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D35" t="n">
         <v>53645015.8526689</v>
@@ -2470,13 +2491,13 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B36" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D36" t="n">
         <v>97558708.5693301</v>
@@ -2496,13 +2517,13 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B37" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C37" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D37" t="n">
         <v>6995153.2264799</v>
@@ -2522,13 +2543,13 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B38" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C38" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D38" t="n">
         <v>5718010.03460558</v>
@@ -2548,13 +2569,13 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B39" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C39" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D39" t="n">
         <v>3371865.93699235</v>
@@ -2574,13 +2595,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B40" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C40" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D40" t="n">
         <v>3073282.08579806</v>
@@ -2600,13 +2621,13 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B41" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C41" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D41" t="n">
         <v>14700122.5324854</v>
@@ -2626,13 +2647,13 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B42" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C42" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D42" t="n">
         <v>55625128.1760766</v>
@@ -2652,13 +2673,13 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B43" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C43" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D43" t="n">
         <v>95135040.149482</v>
@@ -2678,13 +2699,13 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B44" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C44" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D44" t="n">
         <v>125925837.51197</v>
@@ -2704,13 +2725,13 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B45" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C45" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D45" t="n">
         <v>41978645.8917725</v>
@@ -2730,13 +2751,13 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B46" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C46" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D46" t="n">
         <v>30094165.5624909</v>
@@ -2756,13 +2777,13 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B47" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C47" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D47" t="n">
         <v>60002929.9315364</v>
@@ -2782,13 +2803,13 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B48" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C48" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D48" t="n">
         <v>30923237.8879497</v>
@@ -2808,13 +2829,13 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B49" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C49" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D49" t="n">
         <v>18441786.9254095</v>
@@ -2834,13 +2855,13 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B50" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D50" t="n">
         <v>10302411.643222</v>
@@ -2860,13 +2881,13 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B51" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C51" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D51" t="n">
         <v>52098883.1421237</v>
@@ -2886,13 +2907,13 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B52" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C52" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D52" t="n">
         <v>145150311.901617</v>
@@ -2912,13 +2933,13 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B53" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C53" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D53" t="n">
         <v>139275397.11224</v>
@@ -2938,13 +2959,13 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B54" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C54" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D54" t="n">
         <v>1906664.22502504</v>
@@ -2964,13 +2985,13 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B55" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C55" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D55" t="n">
         <v>1841886.6432806</v>
@@ -2990,13 +3011,13 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B56" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C56" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D56" t="n">
         <v>129575381.16787</v>
@@ -3016,13 +3037,13 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B57" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C57" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D57" t="n">
         <v>1011804.19332115</v>
@@ -3042,13 +3063,13 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B58" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C58" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D58" t="n">
         <v>45657260.703393</v>
@@ -3068,13 +3089,13 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B59" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C59" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D59" t="n">
         <v>83647549.9222833</v>
@@ -3094,13 +3115,13 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B60" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C60" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D60" t="n">
         <v>195522530.481548</v>
@@ -3120,13 +3141,13 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B61" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C61" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D61" t="n">
         <v>99800668.2195884</v>
@@ -3146,13 +3167,13 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B62" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C62" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D62" t="n">
         <v>13103156.2849833</v>
@@ -3172,13 +3193,13 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B63" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C63" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D63" t="n">
         <v>11063602.4607723</v>
@@ -3198,13 +3219,13 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
+        <v>157</v>
+      </c>
+      <c r="B64" t="s">
+        <v>159</v>
+      </c>
+      <c r="C64" t="s">
         <v>155</v>
-      </c>
-      <c r="B64" t="s">
-        <v>157</v>
-      </c>
-      <c r="C64" t="s">
-        <v>153</v>
       </c>
       <c r="D64" t="n">
         <v>64005713.317842</v>
@@ -3224,13 +3245,13 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B65" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C65" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D65" t="n">
         <v>5964288.80316966</v>
@@ -3250,13 +3271,13 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B66" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C66" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D66" t="n">
         <v>38868660.2581769</v>
@@ -3276,13 +3297,13 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B67" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C67" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D67" t="n">
         <v>30652653.6705294</v>
@@ -3302,13 +3323,13 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B68" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C68" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D68" t="n">
         <v>77739229.9485382</v>
@@ -3328,13 +3349,13 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B69" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C69" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D69" t="n">
         <v>91325766.613322</v>
@@ -3354,13 +3375,13 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B70" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C70" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D70" t="n">
         <v>13440549.3542245</v>
@@ -3380,13 +3401,13 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B71" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C71" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D71" t="n">
         <v>18941417.5996459</v>
@@ -3406,13 +3427,13 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B72" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C72" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D72" t="n">
         <v>17635406.6271994</v>
@@ -3432,13 +3453,13 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B73" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C73" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D73" t="n">
         <v>19968969.3874486</v>
@@ -3458,13 +3479,13 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B74" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C74" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D74" t="n">
         <v>10656439.170699</v>
@@ -3484,13 +3505,13 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B75" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C75" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D75" t="n">
         <v>43196255.717706</v>
@@ -3510,13 +3531,13 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B76" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C76" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D76" t="n">
         <v>24545802.8927485</v>
@@ -3536,13 +3557,13 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B77" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C77" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D77" t="n">
         <v>11010484.4895777</v>
@@ -3562,13 +3583,13 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B78" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C78" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D78" t="n">
         <v>149274616.881634</v>
@@ -3588,13 +3609,13 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B79" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C79" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D79" t="n">
         <v>59818952.0627199</v>
@@ -3614,13 +3635,13 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B80" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C80" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D80" t="n">
         <v>8596263.16560653</v>
@@ -3640,13 +3661,13 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B81" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C81" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D81" t="n">
         <v>3418574.09223901</v>
@@ -3666,13 +3687,13 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B82" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C82" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D82" t="n">
         <v>52160876.1644732</v>
@@ -3692,13 +3713,13 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B83" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C83" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D83" t="n">
         <v>22752724.4509174</v>
@@ -3718,13 +3739,13 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B84" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C84" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D84" t="n">
         <v>67619348.3070889</v>
@@ -3744,13 +3765,13 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B85" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C85" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D85" t="n">
         <v>49526041.5691039</v>
@@ -3770,13 +3791,13 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B86" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C86" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D86" t="n">
         <v>65919104.3941101</v>
@@ -3796,13 +3817,13 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B87" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C87" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D87" t="n">
         <v>34923124.7304491</v>
@@ -3822,13 +3843,13 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B88" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C88" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D88" t="n">
         <v>7057604.73748038</v>
@@ -3848,13 +3869,13 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B89" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C89" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D89" t="n">
         <v>7517153.66999239</v>
@@ -3874,13 +3895,13 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B90" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C90" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D90" t="n">
         <v>61137887.2072945</v>
@@ -3900,13 +3921,13 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B91" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C91" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D91" t="n">
         <v>21249077.9153833</v>
@@ -3926,13 +3947,13 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B92" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C92" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D92" t="n">
         <v>4671207.48403612</v>
@@ -3952,13 +3973,13 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B93" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C93" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D93" t="n">
         <v>4069358.80125304</v>
@@ -3978,13 +3999,13 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B94" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C94" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D94" t="n">
         <v>8482835.59893755</v>
@@ -4004,13 +4025,13 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B95" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C95" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D95" t="n">
         <v>5845907.5068317</v>
@@ -4030,13 +4051,13 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B96" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C96" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D96" t="n">
         <v>4462320.18601146</v>
@@ -4056,13 +4077,13 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B97" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C97" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D97" t="n">
         <v>3632964.20437794</v>
@@ -4082,13 +4103,13 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B98" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C98" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D98" t="n">
         <v>11643739.595004</v>
@@ -4108,13 +4129,13 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B99" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C99" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D99" t="n">
         <v>3089412.12774896</v>
@@ -4134,13 +4155,13 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B100" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C100" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D100" t="n">
         <v>9319727.83006421</v>
@@ -4160,13 +4181,13 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B101" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C101" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D101" t="n">
         <v>28337989.1618802</v>
@@ -4186,13 +4207,13 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B102" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C102" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D102" t="n">
         <v>8968868.94812895</v>
@@ -4212,13 +4233,13 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B103" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C103" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D103" t="n">
         <v>13562125.3932083</v>
@@ -4238,13 +4259,13 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B104" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C104" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D104" t="n">
         <v>8987110.10581461</v>
@@ -4264,13 +4285,13 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B105" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C105" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D105" t="n">
         <v>1598782.64733342</v>
@@ -4290,13 +4311,13 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B106" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C106" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D106" t="n">
         <v>1757556.43463122</v>
@@ -4316,13 +4337,13 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B107" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C107" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D107" t="n">
         <v>2467483.60943227</v>
@@ -4342,13 +4363,13 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B108" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C108" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D108" t="n">
         <v>6759100.11540427</v>
@@ -4368,13 +4389,13 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B109" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C109" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D109" t="n">
         <v>191700.511288392</v>
@@ -4394,13 +4415,13 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B110" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C110" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D110" t="n">
         <v>4123396.60954736</v>
@@ -4420,13 +4441,13 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B111" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C111" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D111" t="n">
         <v>136383454.068239</v>
@@ -4446,13 +4467,13 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B112" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C112" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D112" t="n">
         <v>1706433.59602305</v>
@@ -4472,13 +4493,13 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B113" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C113" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D113" t="n">
         <v>4721484.41819194</v>
@@ -4498,13 +4519,13 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B114" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C114" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D114" t="n">
         <v>6473.10475685959</v>
@@ -4524,13 +4545,13 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B115" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C115" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D115" t="n">
         <v>1017169.27188582</v>
@@ -4550,13 +4571,13 @@
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B116" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C116" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D116" t="n">
         <v>1398929.63092605</v>
@@ -4576,13 +4597,13 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B117" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C117" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D117" t="n">
         <v>2319996.53830937</v>
@@ -4602,13 +4623,13 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B118" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C118" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D118" t="n">
         <v>0</v>
@@ -4628,13 +4649,13 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B119" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C119" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D119" t="n">
         <v>5551959.86410522</v>
@@ -4654,13 +4675,13 @@
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B120" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C120" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D120" t="n">
         <v>2877106.3681012</v>
@@ -4680,13 +4701,13 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B121" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C121" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D121" t="n">
         <v>3902410.09273463</v>
@@ -4706,13 +4727,13 @@
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B122" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C122" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D122" t="n">
         <v>146118485.754537</v>
@@ -4732,13 +4753,13 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B123" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C123" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D123" t="n">
         <v>0</v>
@@ -4758,13 +4779,13 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B124" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C124" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D124" t="n">
         <v>2749799.78212351</v>
@@ -4784,13 +4805,13 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B125" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C125" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D125" t="n">
         <v>2826166.65493782</v>
@@ -4810,13 +4831,13 @@
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B126" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C126" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D126" t="n">
         <v>8273920.55887713</v>
@@ -4836,13 +4857,13 @@
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B127" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C127" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D127" t="n">
         <v>683475.139183399</v>
@@ -4862,13 +4883,13 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B128" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C128" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D128" t="n">
         <v>9441679.39642369</v>
@@ -4888,13 +4909,13 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B129" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C129" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D129" t="n">
         <v>627339.235001181</v>
@@ -4914,13 +4935,13 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B130" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C130" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D130" t="n">
         <v>49122506.0354811</v>
@@ -4940,13 +4961,13 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B131" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C131" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D131" t="n">
         <v>11895926.1250244</v>
@@ -4966,13 +4987,13 @@
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B132" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C132" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D132" t="n">
         <v>2329652.02535391</v>
@@ -4992,13 +5013,13 @@
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B133" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C133" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D133" t="n">
         <v>1453911.61007745</v>
@@ -5018,13 +5039,13 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B134" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C134" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D134" t="n">
         <v>58617225.6902096</v>
@@ -5044,13 +5065,13 @@
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B135" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C135" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D135" t="n">
         <v>12902240.3988501</v>
@@ -5070,13 +5091,13 @@
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B136" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C136" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D136" t="n">
         <v>364022.37957393</v>
@@ -5096,13 +5117,13 @@
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B137" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C137" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D137" t="n">
         <v>35544146.9005234</v>
@@ -5122,13 +5143,13 @@
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B138" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C138" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D138" t="n">
         <v>2023626.79874268</v>
@@ -5148,13 +5169,13 @@
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B139" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C139" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D139" t="n">
         <v>4008735.33709944</v>
@@ -5174,13 +5195,13 @@
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B140" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C140" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D140" t="n">
         <v>296208.602517667</v>
@@ -5200,13 +5221,13 @@
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B141" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C141" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D141" t="n">
         <v>42682.4164538815</v>
@@ -5226,13 +5247,13 @@
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B142" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C142" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D142" t="n">
         <v>1602184.99926922</v>
@@ -5252,13 +5273,13 @@
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B143" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C143" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D143" t="n">
         <v>23320916.9593411</v>
@@ -5278,13 +5299,13 @@
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B144" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C144" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D144" t="n">
         <v>10839119.7396974</v>
@@ -5304,13 +5325,13 @@
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B145" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C145" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D145" t="n">
         <v>2155159.8809871</v>
@@ -5330,13 +5351,13 @@
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B146" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C146" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D146" t="n">
         <v>20782056.7734799</v>
@@ -5356,13 +5377,13 @@
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B147" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C147" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D147" t="n">
         <v>31620725.2845488</v>
@@ -5382,13 +5403,13 @@
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B148" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C148" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D148" t="n">
         <v>4316311.10255573</v>
@@ -5408,13 +5429,13 @@
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B149" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C149" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D149" t="n">
         <v>4003251.59622488</v>
@@ -5434,13 +5455,13 @@
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B150" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C150" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D150" t="n">
         <v>27704575.2652053</v>
@@ -5460,13 +5481,13 @@
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B151" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C151" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D151" t="n">
         <v>4485148.86196108</v>
@@ -5486,13 +5507,13 @@
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B152" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C152" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D152" t="n">
         <v>8789726.10713858</v>
@@ -5512,13 +5533,13 @@
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B153" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C153" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D153" t="n">
         <v>6672085.1809307</v>
@@ -5538,13 +5559,13 @@
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B154" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C154" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D154" t="n">
         <v>11118716.3975415</v>
@@ -5564,13 +5585,13 @@
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B155" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C155" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D155" t="n">
         <v>3673477.73077899</v>
@@ -5590,13 +5611,13 @@
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B156" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C156" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D156" t="n">
         <v>12342198.3533143</v>
@@ -5616,13 +5637,13 @@
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B157" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C157" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D157" t="n">
         <v>13419980.3041932</v>
@@ -5642,13 +5663,13 @@
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B158" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C158" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D158" t="n">
         <v>3799871.71887914</v>
@@ -5668,13 +5689,13 @@
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B159" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C159" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D159" t="n">
         <v>4104962.95137674</v>
@@ -5694,13 +5715,13 @@
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B160" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C160" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D160" t="n">
         <v>2314329.46141835</v>
@@ -5720,13 +5741,13 @@
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B161" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C161" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D161" t="n">
         <v>0</v>
@@ -5746,13 +5767,13 @@
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B162" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C162" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D162" t="n">
         <v>15581.9795453705</v>
@@ -5772,13 +5793,13 @@
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B163" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C163" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D163" t="n">
         <v>15581.9795453705</v>
@@ -5798,13 +5819,13 @@
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B164" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C164" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D164" t="n">
         <v>3785.47394239446</v>
@@ -5824,13 +5845,13 @@
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B165" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C165" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D165" t="n">
         <v>64164869.0224339</v>
@@ -5850,13 +5871,13 @@
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B166" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C166" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D166" t="n">
         <v>0</v>
@@ -5876,13 +5897,13 @@
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B167" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C167" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D167" t="n">
         <v>16710204.8402737</v>
@@ -5902,13 +5923,13 @@
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B168" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C168" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D168" t="n">
         <v>938581.888958131</v>
@@ -5928,13 +5949,13 @@
     </row>
     <row r="169">
       <c r="A169" t="s">
+        <v>211</v>
+      </c>
+      <c r="B169" t="s">
+        <v>159</v>
+      </c>
+      <c r="C169" t="s">
         <v>209</v>
-      </c>
-      <c r="B169" t="s">
-        <v>157</v>
-      </c>
-      <c r="C169" t="s">
-        <v>207</v>
       </c>
       <c r="D169" t="n">
         <v>30331488.2013504</v>
@@ -5954,13 +5975,13 @@
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B170" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C170" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D170" t="n">
         <v>26467834.256642</v>
@@ -5980,13 +6001,13 @@
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B171" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C171" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D171" t="n">
         <v>10901763.1756963</v>
@@ -6006,13 +6027,13 @@
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B172" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C172" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D172" t="n">
         <v>1771710.24569029</v>
@@ -6032,13 +6053,13 @@
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B173" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C173" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D173" t="n">
         <v>3241679.94717261</v>
@@ -6058,13 +6079,13 @@
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B174" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C174" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D174" t="n">
         <v>41586486.6099352</v>
@@ -6084,13 +6105,13 @@
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B175" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C175" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D175" t="n">
         <v>24650980.2913871</v>
@@ -6110,13 +6131,13 @@
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B176" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C176" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D176" t="n">
         <v>9099683.21874044</v>
@@ -6136,13 +6157,13 @@
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B177" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C177" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D177" t="n">
         <v>4355775.70762582</v>
@@ -6162,13 +6183,13 @@
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B178" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C178" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D178" t="n">
         <v>32702023.7168979</v>
@@ -6188,13 +6209,13 @@
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B179" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C179" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D179" t="n">
         <v>1182612.51110831</v>
@@ -6214,13 +6235,13 @@
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B180" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C180" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D180" t="n">
         <v>1852929.03483688</v>
@@ -6240,13 +6261,13 @@
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B181" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C181" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D181" t="n">
         <v>325912.4234083</v>
@@ -6266,13 +6287,13 @@
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B182" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C182" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D182" t="n">
         <v>3000344.1203645</v>
@@ -6292,13 +6313,13 @@
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B183" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C183" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D183" t="n">
         <v>1228860.98101177</v>
@@ -6318,13 +6339,13 @@
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B184" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C184" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D184" t="n">
         <v>1861902.30084203</v>
@@ -6344,13 +6365,13 @@
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B185" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C185" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D185" t="n">
         <v>4641376.88080348</v>
@@ -6370,13 +6391,13 @@
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B186" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C186" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D186" t="n">
         <v>20035750.0414657</v>
@@ -6396,13 +6417,13 @@
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B187" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C187" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D187" t="n">
         <v>39026894.4790605</v>
@@ -6422,13 +6443,13 @@
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B188" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C188" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D188" t="n">
         <v>802967.419651324</v>
@@ -6448,13 +6469,13 @@
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B189" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C189" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D189" t="n">
         <v>35684910.7335826</v>
@@ -6474,13 +6495,13 @@
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B190" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C190" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D190" t="n">
         <v>8363554.45706136</v>
@@ -6500,13 +6521,13 @@
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B191" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C191" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D191" t="n">
         <v>8912907.85073428</v>
@@ -6526,13 +6547,13 @@
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B192" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C192" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D192" t="n">
         <v>10475102.8854975</v>
@@ -6552,13 +6573,13 @@
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B193" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C193" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D193" t="n">
         <v>1474840.94437476</v>
@@ -6578,13 +6599,13 @@
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B194" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C194" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D194" t="n">
         <v>3976543.53491912</v>
@@ -6604,13 +6625,13 @@
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B195" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C195" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D195" t="n">
         <v>2459573.81610199</v>
@@ -6630,13 +6651,13 @@
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B196" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C196" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D196" t="n">
         <v>2282315.18630685</v>
@@ -6656,13 +6677,13 @@
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B197" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C197" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D197" t="n">
         <v>7364887.72448074</v>
@@ -6682,13 +6703,13 @@
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B198" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C198" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D198" t="n">
         <v>2583682.11846957</v>
@@ -6708,13 +6729,13 @@
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B199" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C199" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D199" t="n">
         <v>41667972.2101032</v>
@@ -6734,13 +6755,13 @@
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B200" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C200" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D200" t="n">
         <v>2676740.8016228</v>
@@ -6760,13 +6781,13 @@
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B201" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C201" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D201" t="n">
         <v>50936565.4560885</v>
@@ -6786,13 +6807,13 @@
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B202" t="s">
+        <v>159</v>
+      </c>
+      <c r="C202" t="s">
         <v>157</v>
-      </c>
-      <c r="C202" t="s">
-        <v>155</v>
       </c>
       <c r="D202" t="n">
         <v>389516203.233821</v>
@@ -6812,13 +6833,13 @@
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B203" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C203" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D203" t="n">
         <v>9803755.58879593</v>
@@ -6838,13 +6859,13 @@
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B204" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C204" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D204" t="n">
         <v>6859279.99449494</v>
@@ -6864,13 +6885,13 @@
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B205" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C205" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D205" t="n">
         <v>0</v>
@@ -6890,13 +6911,13 @@
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B206" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C206" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D206" t="n">
         <v>616068.247335644</v>
@@ -6916,13 +6937,13 @@
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B207" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C207" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D207" t="n">
         <v>45467023.8241105</v>
@@ -6942,13 +6963,13 @@
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B208" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C208" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D208" t="n">
         <v>45467023.8241105</v>
@@ -6968,13 +6989,13 @@
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B209" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C209" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D209" t="n">
         <v>338279.830848863</v>
@@ -7008,27 +7029,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B2" t="n">
         <v>1957056508.54051</v>
@@ -7048,7 +7069,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B3" t="n">
         <v>4244549770.95737</v>
@@ -7068,7 +7089,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B4" t="n">
         <v>660381823</v>
@@ -7088,7 +7109,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B5" t="n">
         <v>530228764</v>
@@ -7108,7 +7129,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B6" t="n">
         <v>7491859197.68968</v>
@@ -7128,7 +7149,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B7" t="n">
         <v>7078021722.42879</v>
@@ -7148,7 +7169,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B8" t="n">
         <v>2137155596.94256</v>
@@ -7168,7 +7189,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B9" t="n">
         <v>863281732</v>

</xml_diff>

<commit_message>
updated for R 3.6.2
</commit_message>
<xml_diff>
--- a/out/profiles.xlsx
+++ b/out/profiles.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="pop" sheetId="24" state="visible" r:id="rId2"/>
-    <sheet name="cpi" sheetId="25" state="visible" r:id="rId3"/>
-    <sheet name="avgSpendPicnic" sheetId="26" state="visible" r:id="rId4"/>
-    <sheet name="spend" sheetId="27" state="visible" r:id="rId5"/>
-    <sheet name="spendAll" sheetId="28" state="visible" r:id="rId6"/>
+    <sheet name="pop" sheetId="29" state="visible" r:id="rId2"/>
+    <sheet name="cpi" sheetId="30" state="visible" r:id="rId3"/>
+    <sheet name="avgSpendPicnic" sheetId="31" state="visible" r:id="rId4"/>
+    <sheet name="spend" sheetId="32" state="visible" r:id="rId5"/>
+    <sheet name="spendAll" sheetId="33" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -801,17 +802,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1124,40 +1125,40 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1171,7 +1172,7 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1182,7 +1183,7 @@
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1193,7 +1194,7 @@
       <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1204,7 +1205,7 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1215,19 +1216,19 @@
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>